<commit_message>
Updated beena Nov16 ExcelLib
</commit_message>
<xml_diff>
--- a/src/test/resources/BBTestDataNew.xlsx
+++ b/src/test/resources/BBTestDataNew.xlsx
@@ -131,8 +131,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -160,56 +164,61 @@
   <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>8553331269</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>78</v>
       </c>
     </row>

</xml_diff>